<commit_message>
added rud per capita and changed the extrapolation calculation
</commit_message>
<xml_diff>
--- a/graphs/graf_2a.xlsx
+++ b/graphs/graf_2a.xlsx
@@ -460,7 +460,7 @@
         <v>15778.01799808131</v>
       </c>
       <c r="C2" t="n">
-        <v>655873.0192802602</v>
+        <v>636733.2941520028</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>14627.79040287244</v>
       </c>
       <c r="C3" t="n">
-        <v>641321.727382406</v>
+        <v>622606.6389124633</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>14218.80066201299</v>
       </c>
       <c r="C4" t="n">
-        <v>459353.0684396127</v>
+        <v>445948.2001064043</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>13206.02814051673</v>
       </c>
       <c r="C5" t="n">
-        <v>651176.511234998</v>
+        <v>632173.8398814903</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>12865.11888801059</v>
       </c>
       <c r="C6" t="n">
-        <v>664831.4081950632</v>
+        <v>645430.2588331797</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>11860.42295982869</v>
       </c>
       <c r="C7" t="n">
-        <v>594307.8991303849</v>
+        <v>576964.7709690979</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +538,7 @@
         <v>11645.88975371437</v>
       </c>
       <c r="C8" t="n">
-        <v>618665.0409249018</v>
+        <v>600611.1212153231</v>
       </c>
     </row>
     <row r="9">
@@ -551,7 +551,7 @@
         <v>11552.01063969364</v>
       </c>
       <c r="C9" t="n">
-        <v>551692.8635761528</v>
+        <v>535593.3298955993</v>
       </c>
     </row>
     <row r="10">
@@ -564,7 +564,7 @@
         <v>11272.87044389844</v>
       </c>
       <c r="C10" t="n">
-        <v>557760.4844923652</v>
+        <v>541483.8851404014</v>
       </c>
     </row>
     <row r="11">
@@ -577,7 +577,7 @@
         <v>10556.85866039842</v>
       </c>
       <c r="C11" t="n">
-        <v>675993.2943994324</v>
+        <v>656266.418216069</v>
       </c>
     </row>
     <row r="12">
@@ -590,7 +590,7 @@
         <v>10047.99075472575</v>
       </c>
       <c r="C12" t="n">
-        <v>631535.6036805105</v>
+        <v>613106.0944495659</v>
       </c>
     </row>
     <row r="13">
@@ -603,7 +603,7 @@
         <v>8988.948359037528</v>
       </c>
       <c r="C13" t="n">
-        <v>595473.4701864539</v>
+        <v>578096.3282618701</v>
       </c>
     </row>
     <row r="14">
@@ -616,7 +616,7 @@
         <v>8657.428677942709</v>
       </c>
       <c r="C14" t="n">
-        <v>734286.6653226282</v>
+        <v>712858.6685511762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>